<commit_message>
fix: corrected missing JPTL
</commit_message>
<xml_diff>
--- a/UNDER DEVELOPMENT/JFACC/OPAR_JOINT_TARGET_LIST_D1.xlsx
+++ b/UNDER DEVELOPMENT/JFACC/OPAR_JOINT_TARGET_LIST_D1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Target List" sheetId="1" r:id="rId1"/>
@@ -2896,7 +2896,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="156">
+  <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -3204,6 +3204,84 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -3228,111 +3306,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3350,6 +3350,12 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3389,7 +3395,7 @@
         <xdr:cNvPr id="2" name="Bilde 1" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3434,7 +3440,7 @@
         <xdr:cNvPr id="3" name="Bilde 2" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3484,7 +3490,7 @@
         <xdr:cNvPr id="2" name="Bilde 1" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3529,7 +3535,7 @@
         <xdr:cNvPr id="3" name="Bilde 2" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3579,7 +3585,7 @@
         <xdr:cNvPr id="2" name="Bilde 1" descr="Patch_wip3.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3624,7 +3630,7 @@
         <xdr:cNvPr id="3" name="Bilde 2" descr="OPAR JFACC logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3674,7 +3680,7 @@
         <xdr:cNvPr id="4" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3727,7 +3733,7 @@
         <xdr:cNvPr id="3" name="TekstSylinder 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3819,7 +3825,7 @@
         <xdr:cNvPr id="2049" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000001080000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000001080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3877,7 +3883,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3930,7 +3936,7 @@
         <xdr:cNvPr id="2049" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000001080000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000001080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3983,7 +3989,7 @@
         <xdr:cNvPr id="4" name="TekstSylinder 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4081,7 +4087,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4134,7 +4140,7 @@
         <xdr:cNvPr id="4" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4187,7 +4193,7 @@
         <xdr:cNvPr id="5" name="TekstSylinder 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4281,7 +4287,7 @@
         <xdr:cNvPr id="5" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4334,7 +4340,7 @@
         <xdr:cNvPr id="6" name="TekstSylinder 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4429,7 +4435,7 @@
         <xdr:cNvPr id="4" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4487,7 +4493,7 @@
         <xdr:cNvPr id="3073" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-0000010C0000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000010C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4540,7 +4546,7 @@
         <xdr:cNvPr id="3074" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-0000020C0000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000020C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4593,7 +4599,7 @@
         <xdr:cNvPr id="3075" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-0000030C0000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000030C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4646,7 +4652,7 @@
         <xdr:cNvPr id="3076" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-0000040C0000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000040C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4699,7 +4705,7 @@
         <xdr:cNvPr id="3077" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-0000050C0000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000050C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4752,7 +4758,7 @@
         <xdr:cNvPr id="3078" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-0000060C0000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000060C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4805,7 +4811,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000001040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5131,8 +5137,8 @@
   <dimension ref="A1:H317"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B64" sqref="B64"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -9767,8 +9773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -9785,50 +9791,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="49.9" customHeight="1">
-      <c r="A1" s="130" t="s">
+      <c r="A1" s="107" t="s">
         <v>561</v>
       </c>
-      <c r="B1" s="131"/>
-      <c r="C1" s="131"/>
-      <c r="D1" s="131"/>
-      <c r="E1" s="131"/>
-      <c r="F1" s="131"/>
-      <c r="G1" s="131"/>
-      <c r="H1" s="131"/>
-      <c r="I1" s="132"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="108"/>
+      <c r="I1" s="109"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A2" s="133" t="s">
+      <c r="A2" s="110" t="s">
         <v>562</v>
       </c>
-      <c r="B2" s="134"/>
+      <c r="B2" s="111"/>
       <c r="C2" s="18" t="s">
         <v>563</v>
       </c>
-      <c r="D2" s="137" t="s">
+      <c r="D2" s="114" t="s">
         <v>564</v>
       </c>
-      <c r="E2" s="138"/>
-      <c r="F2" s="138"/>
-      <c r="G2" s="139"/>
-      <c r="H2" s="135" t="s">
+      <c r="E2" s="115"/>
+      <c r="F2" s="115"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="112" t="s">
         <v>565</v>
       </c>
-      <c r="I2" s="136"/>
+      <c r="I2" s="113"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickBot="1"/>
     <row r="4" spans="1:9" ht="15.75">
-      <c r="A4" s="140" t="s">
+      <c r="A4" s="117" t="s">
         <v>566</v>
       </c>
-      <c r="B4" s="141"/>
-      <c r="C4" s="141"/>
-      <c r="D4" s="141"/>
-      <c r="E4" s="141"/>
-      <c r="F4" s="141"/>
-      <c r="G4" s="141"/>
-      <c r="H4" s="141"/>
-      <c r="I4" s="142"/>
+      <c r="B4" s="118"/>
+      <c r="C4" s="118"/>
+      <c r="D4" s="118"/>
+      <c r="E4" s="118"/>
+      <c r="F4" s="118"/>
+      <c r="G4" s="118"/>
+      <c r="H4" s="118"/>
+      <c r="I4" s="119"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1">
       <c r="A5" s="97" t="s">
@@ -9863,7 +9869,7 @@
       <c r="A6" s="100">
         <v>1</v>
       </c>
-      <c r="B6" s="101" t="s">
+      <c r="B6" s="156" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="101" t="s">
@@ -9892,7 +9898,7 @@
       <c r="A7" s="9">
         <v>2</v>
       </c>
-      <c r="B7" s="95" t="s">
+      <c r="B7" s="157" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="95" t="s">
@@ -10093,17 +10099,17 @@
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" ht="15.75">
-      <c r="A15" s="119" t="s">
+      <c r="A15" s="120" t="s">
         <v>591</v>
       </c>
-      <c r="B15" s="120"/>
-      <c r="C15" s="120"/>
-      <c r="D15" s="120"/>
-      <c r="E15" s="120"/>
-      <c r="F15" s="120"/>
-      <c r="G15" s="120"/>
-      <c r="H15" s="120"/>
-      <c r="I15" s="121"/>
+      <c r="B15" s="121"/>
+      <c r="C15" s="121"/>
+      <c r="D15" s="121"/>
+      <c r="E15" s="121"/>
+      <c r="F15" s="121"/>
+      <c r="G15" s="121"/>
+      <c r="H15" s="121"/>
+      <c r="I15" s="122"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="6" t="s">
@@ -10118,15 +10124,15 @@
       <c r="D16" s="4" t="s">
         <v>573</v>
       </c>
-      <c r="E16" s="122" t="s">
+      <c r="E16" s="125" t="s">
         <v>592</v>
       </c>
-      <c r="F16" s="128"/>
-      <c r="G16" s="122" t="s">
+      <c r="F16" s="131"/>
+      <c r="G16" s="125" t="s">
         <v>593</v>
       </c>
-      <c r="H16" s="123"/>
-      <c r="I16" s="124"/>
+      <c r="H16" s="126"/>
+      <c r="I16" s="127"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="7">
@@ -10141,15 +10147,15 @@
       <c r="D17" s="103" t="s">
         <v>578</v>
       </c>
-      <c r="E17" s="125" t="s">
+      <c r="E17" s="128" t="s">
         <v>595</v>
       </c>
-      <c r="F17" s="129"/>
-      <c r="G17" s="125" t="s">
+      <c r="F17" s="132"/>
+      <c r="G17" s="128" t="s">
         <v>596</v>
       </c>
-      <c r="H17" s="126"/>
-      <c r="I17" s="127"/>
+      <c r="H17" s="129"/>
+      <c r="I17" s="130"/>
     </row>
     <row r="18" spans="1:9" ht="30">
       <c r="A18" s="7">
@@ -10164,15 +10170,15 @@
       <c r="D18" s="103" t="s">
         <v>587</v>
       </c>
-      <c r="E18" s="125" t="s">
+      <c r="E18" s="128" t="s">
         <v>595</v>
       </c>
-      <c r="F18" s="129"/>
-      <c r="G18" s="125" t="s">
+      <c r="F18" s="132"/>
+      <c r="G18" s="128" t="s">
         <v>598</v>
       </c>
-      <c r="H18" s="126"/>
-      <c r="I18" s="127"/>
+      <c r="H18" s="129"/>
+      <c r="I18" s="130"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="7">
@@ -10187,13 +10193,13 @@
       <c r="D19" s="103" t="s">
         <v>589</v>
       </c>
-      <c r="E19" s="125" t="s">
+      <c r="E19" s="128" t="s">
         <v>595</v>
       </c>
-      <c r="F19" s="129"/>
-      <c r="G19" s="125"/>
-      <c r="H19" s="126"/>
-      <c r="I19" s="127"/>
+      <c r="F19" s="132"/>
+      <c r="G19" s="128"/>
+      <c r="H19" s="129"/>
+      <c r="I19" s="130"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="7">
@@ -10208,13 +10214,13 @@
       <c r="D20" s="103" t="s">
         <v>589</v>
       </c>
-      <c r="E20" s="125" t="s">
+      <c r="E20" s="128" t="s">
         <v>595</v>
       </c>
-      <c r="F20" s="129"/>
-      <c r="G20" s="125"/>
-      <c r="H20" s="126"/>
-      <c r="I20" s="127"/>
+      <c r="F20" s="132"/>
+      <c r="G20" s="128"/>
+      <c r="H20" s="129"/>
+      <c r="I20" s="130"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="7">
@@ -10223,11 +10229,11 @@
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
-      <c r="E21" s="115"/>
-      <c r="F21" s="118"/>
-      <c r="G21" s="115"/>
-      <c r="H21" s="116"/>
-      <c r="I21" s="117"/>
+      <c r="E21" s="123"/>
+      <c r="F21" s="124"/>
+      <c r="G21" s="123"/>
+      <c r="H21" s="141"/>
+      <c r="I21" s="142"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="7">
@@ -10236,11 +10242,11 @@
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
-      <c r="E22" s="115"/>
-      <c r="F22" s="118"/>
-      <c r="G22" s="115"/>
-      <c r="H22" s="116"/>
-      <c r="I22" s="117"/>
+      <c r="E22" s="123"/>
+      <c r="F22" s="124"/>
+      <c r="G22" s="123"/>
+      <c r="H22" s="141"/>
+      <c r="I22" s="142"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="7">
@@ -10249,11 +10255,11 @@
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
-      <c r="E23" s="115"/>
-      <c r="F23" s="118"/>
-      <c r="G23" s="115"/>
-      <c r="H23" s="116"/>
-      <c r="I23" s="117"/>
+      <c r="E23" s="123"/>
+      <c r="F23" s="124"/>
+      <c r="G23" s="123"/>
+      <c r="H23" s="141"/>
+      <c r="I23" s="142"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="7">
@@ -10262,11 +10268,11 @@
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
-      <c r="E24" s="115"/>
-      <c r="F24" s="118"/>
-      <c r="G24" s="115"/>
-      <c r="H24" s="116"/>
-      <c r="I24" s="117"/>
+      <c r="E24" s="123"/>
+      <c r="F24" s="124"/>
+      <c r="G24" s="123"/>
+      <c r="H24" s="141"/>
+      <c r="I24" s="142"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="7">
@@ -10275,11 +10281,11 @@
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
-      <c r="E25" s="107"/>
-      <c r="F25" s="108"/>
-      <c r="G25" s="107"/>
-      <c r="H25" s="109"/>
-      <c r="I25" s="110"/>
+      <c r="E25" s="133"/>
+      <c r="F25" s="134"/>
+      <c r="G25" s="133"/>
+      <c r="H25" s="135"/>
+      <c r="I25" s="136"/>
     </row>
     <row r="26" spans="1:9" ht="15.75" thickBot="1">
       <c r="A26" s="8">
@@ -10288,19 +10294,23 @@
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
-      <c r="E26" s="111"/>
-      <c r="F26" s="112"/>
-      <c r="G26" s="111"/>
-      <c r="H26" s="113"/>
-      <c r="I26" s="114"/>
+      <c r="E26" s="137"/>
+      <c r="F26" s="138"/>
+      <c r="G26" s="137"/>
+      <c r="H26" s="139"/>
+      <c r="I26" s="140"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="E24:F24"/>
     <mergeCell ref="A15:I15"/>
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="E23:F23"/>
@@ -10315,19 +10325,19 @@
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="A4:I4"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B7" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -10352,50 +10362,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="49.9" customHeight="1">
-      <c r="A1" s="130" t="s">
+      <c r="A1" s="107" t="s">
         <v>561</v>
       </c>
-      <c r="B1" s="131"/>
-      <c r="C1" s="131"/>
-      <c r="D1" s="131"/>
-      <c r="E1" s="131"/>
-      <c r="F1" s="131"/>
-      <c r="G1" s="131"/>
-      <c r="H1" s="131"/>
-      <c r="I1" s="132"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="108"/>
+      <c r="I1" s="109"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A2" s="133" t="s">
+      <c r="A2" s="110" t="s">
         <v>562</v>
       </c>
-      <c r="B2" s="134"/>
+      <c r="B2" s="111"/>
       <c r="C2" s="18" t="s">
         <v>601</v>
       </c>
-      <c r="D2" s="137" t="s">
+      <c r="D2" s="114" t="s">
         <v>564</v>
       </c>
-      <c r="E2" s="138"/>
-      <c r="F2" s="138"/>
-      <c r="G2" s="139"/>
-      <c r="H2" s="135" t="s">
+      <c r="E2" s="115"/>
+      <c r="F2" s="115"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="112" t="s">
         <v>602</v>
       </c>
-      <c r="I2" s="136"/>
+      <c r="I2" s="113"/>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1"/>
     <row r="4" spans="1:17" ht="15.75">
-      <c r="A4" s="140" t="s">
+      <c r="A4" s="117" t="s">
         <v>566</v>
       </c>
-      <c r="B4" s="141"/>
-      <c r="C4" s="141"/>
-      <c r="D4" s="141"/>
-      <c r="E4" s="141"/>
-      <c r="F4" s="141"/>
-      <c r="G4" s="141"/>
-      <c r="H4" s="141"/>
-      <c r="I4" s="142"/>
+      <c r="B4" s="118"/>
+      <c r="C4" s="118"/>
+      <c r="D4" s="118"/>
+      <c r="E4" s="118"/>
+      <c r="F4" s="118"/>
+      <c r="G4" s="118"/>
+      <c r="H4" s="118"/>
+      <c r="I4" s="119"/>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="19" t="s">
@@ -10457,15 +10467,15 @@
       <c r="I6" s="11" t="s">
         <v>612</v>
       </c>
-      <c r="K6" s="143" t="s">
+      <c r="K6" s="149" t="s">
         <v>613</v>
       </c>
-      <c r="L6" s="143"/>
-      <c r="M6" s="143"/>
-      <c r="N6" s="143"/>
-      <c r="O6" s="143"/>
-      <c r="P6" s="143"/>
-      <c r="Q6" s="143"/>
+      <c r="L6" s="149"/>
+      <c r="M6" s="149"/>
+      <c r="N6" s="149"/>
+      <c r="O6" s="149"/>
+      <c r="P6" s="149"/>
+      <c r="Q6" s="149"/>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="9">
@@ -10495,15 +10505,15 @@
       <c r="I7" s="11" t="s">
         <v>621</v>
       </c>
-      <c r="K7" s="143" t="s">
+      <c r="K7" s="149" t="s">
         <v>622</v>
       </c>
-      <c r="L7" s="143"/>
-      <c r="M7" s="143"/>
-      <c r="N7" s="143"/>
-      <c r="O7" s="143"/>
-      <c r="P7" s="143"/>
-      <c r="Q7" s="143"/>
+      <c r="L7" s="149"/>
+      <c r="M7" s="149"/>
+      <c r="N7" s="149"/>
+      <c r="O7" s="149"/>
+      <c r="P7" s="149"/>
+      <c r="Q7" s="149"/>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="9">
@@ -10611,17 +10621,17 @@
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:17" ht="15.75">
-      <c r="A15" s="119" t="s">
+      <c r="A15" s="120" t="s">
         <v>591</v>
       </c>
-      <c r="B15" s="120"/>
-      <c r="C15" s="120"/>
-      <c r="D15" s="120"/>
-      <c r="E15" s="120"/>
-      <c r="F15" s="120"/>
-      <c r="G15" s="120"/>
-      <c r="H15" s="120"/>
-      <c r="I15" s="121"/>
+      <c r="B15" s="121"/>
+      <c r="C15" s="121"/>
+      <c r="D15" s="121"/>
+      <c r="E15" s="121"/>
+      <c r="F15" s="121"/>
+      <c r="G15" s="121"/>
+      <c r="H15" s="121"/>
+      <c r="I15" s="122"/>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" s="19" t="s">
@@ -10636,15 +10646,15 @@
       <c r="D16" s="17" t="s">
         <v>573</v>
       </c>
-      <c r="E16" s="148" t="s">
+      <c r="E16" s="143" t="s">
         <v>592</v>
       </c>
-      <c r="F16" s="148"/>
-      <c r="G16" s="148" t="s">
+      <c r="F16" s="143"/>
+      <c r="G16" s="143" t="s">
         <v>593</v>
       </c>
-      <c r="H16" s="148"/>
-      <c r="I16" s="149"/>
+      <c r="H16" s="143"/>
+      <c r="I16" s="144"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="7">
@@ -10659,15 +10669,15 @@
       <c r="D17" s="10" t="s">
         <v>630</v>
       </c>
-      <c r="E17" s="144" t="s">
+      <c r="E17" s="145" t="s">
         <v>632</v>
       </c>
-      <c r="F17" s="145"/>
-      <c r="G17" s="144" t="s">
+      <c r="F17" s="146"/>
+      <c r="G17" s="145" t="s">
         <v>633</v>
       </c>
-      <c r="H17" s="146"/>
-      <c r="I17" s="147"/>
+      <c r="H17" s="147"/>
+      <c r="I17" s="148"/>
     </row>
     <row r="18" spans="1:11" ht="23.25">
       <c r="A18" s="7">
@@ -10682,15 +10692,15 @@
       <c r="D18" s="10" t="s">
         <v>630</v>
       </c>
-      <c r="E18" s="144" t="s">
+      <c r="E18" s="145" t="s">
         <v>632</v>
       </c>
-      <c r="F18" s="145"/>
-      <c r="G18" s="144" t="s">
+      <c r="F18" s="146"/>
+      <c r="G18" s="145" t="s">
         <v>635</v>
       </c>
-      <c r="H18" s="146"/>
-      <c r="I18" s="147"/>
+      <c r="H18" s="147"/>
+      <c r="I18" s="148"/>
     </row>
     <row r="19" spans="1:11" ht="34.5">
       <c r="A19" s="7">
@@ -10705,15 +10715,15 @@
       <c r="D19" s="10" t="s">
         <v>637</v>
       </c>
-      <c r="E19" s="144" t="s">
+      <c r="E19" s="145" t="s">
         <v>638</v>
       </c>
-      <c r="F19" s="145"/>
-      <c r="G19" s="144" t="s">
+      <c r="F19" s="146"/>
+      <c r="G19" s="145" t="s">
         <v>639</v>
       </c>
-      <c r="H19" s="146"/>
-      <c r="I19" s="147"/>
+      <c r="H19" s="147"/>
+      <c r="I19" s="148"/>
       <c r="K19" t="s">
         <v>640</v>
       </c>
@@ -10725,11 +10735,11 @@
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
-      <c r="E20" s="115"/>
-      <c r="F20" s="118"/>
-      <c r="G20" s="115"/>
-      <c r="H20" s="116"/>
-      <c r="I20" s="117"/>
+      <c r="E20" s="123"/>
+      <c r="F20" s="124"/>
+      <c r="G20" s="123"/>
+      <c r="H20" s="141"/>
+      <c r="I20" s="142"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="7">
@@ -10738,11 +10748,11 @@
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
-      <c r="E21" s="115"/>
-      <c r="F21" s="118"/>
-      <c r="G21" s="115"/>
-      <c r="H21" s="116"/>
-      <c r="I21" s="117"/>
+      <c r="E21" s="123"/>
+      <c r="F21" s="124"/>
+      <c r="G21" s="123"/>
+      <c r="H21" s="141"/>
+      <c r="I21" s="142"/>
       <c r="K21" t="s">
         <v>641</v>
       </c>
@@ -10754,11 +10764,11 @@
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
-      <c r="E22" s="115"/>
-      <c r="F22" s="118"/>
-      <c r="G22" s="115"/>
-      <c r="H22" s="116"/>
-      <c r="I22" s="117"/>
+      <c r="E22" s="123"/>
+      <c r="F22" s="124"/>
+      <c r="G22" s="123"/>
+      <c r="H22" s="141"/>
+      <c r="I22" s="142"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="7">
@@ -10767,11 +10777,11 @@
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
-      <c r="E23" s="115"/>
-      <c r="F23" s="118"/>
-      <c r="G23" s="115"/>
-      <c r="H23" s="116"/>
-      <c r="I23" s="117"/>
+      <c r="E23" s="123"/>
+      <c r="F23" s="124"/>
+      <c r="G23" s="123"/>
+      <c r="H23" s="141"/>
+      <c r="I23" s="142"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="7">
@@ -10780,11 +10790,11 @@
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
-      <c r="E24" s="115"/>
-      <c r="F24" s="118"/>
-      <c r="G24" s="115"/>
-      <c r="H24" s="116"/>
-      <c r="I24" s="117"/>
+      <c r="E24" s="123"/>
+      <c r="F24" s="124"/>
+      <c r="G24" s="123"/>
+      <c r="H24" s="141"/>
+      <c r="I24" s="142"/>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="7">
@@ -10793,11 +10803,11 @@
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
       <c r="D25" s="16"/>
-      <c r="E25" s="107"/>
-      <c r="F25" s="108"/>
-      <c r="G25" s="107"/>
-      <c r="H25" s="109"/>
-      <c r="I25" s="110"/>
+      <c r="E25" s="133"/>
+      <c r="F25" s="134"/>
+      <c r="G25" s="133"/>
+      <c r="H25" s="135"/>
+      <c r="I25" s="136"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" thickBot="1">
       <c r="A26" s="8">
@@ -10806,28 +10816,14 @@
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
-      <c r="E26" s="111"/>
-      <c r="F26" s="112"/>
-      <c r="G26" s="111"/>
-      <c r="H26" s="113"/>
-      <c r="I26" s="114"/>
+      <c r="E26" s="137"/>
+      <c r="F26" s="138"/>
+      <c r="G26" s="137"/>
+      <c r="H26" s="139"/>
+      <c r="I26" s="140"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:I19"/>
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="G26:I26"/>
     <mergeCell ref="K6:Q6"/>
@@ -10844,6 +10840,20 @@
     <mergeCell ref="G25:I25"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="G20:I20"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:I21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>